<commit_message>
update download method, create interface for future sheet creator
</commit_message>
<xml_diff>
--- a/TrackAnalyser/TrackAnalyser/wwwroot/excel/Admin.xlsx
+++ b/TrackAnalyser/TrackAnalyser/wwwroot/excel/Admin.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Chars</t>
   </si>
@@ -23,13 +23,100 @@
     <t>Iron Maiden</t>
   </si>
   <si>
+    <t>AntRadio</t>
+  </si>
+  <si>
+    <t>20.07.2020 02:10:30</t>
+  </si>
+  <si>
+    <t>04:32</t>
+  </si>
+  <si>
+    <t>Aces High</t>
+  </si>
+  <si>
+    <t>RadioS</t>
+  </si>
+  <si>
+    <t>19.07.2020 02:20:20</t>
+  </si>
+  <si>
+    <t>20.07.2020 02:12:30</t>
+  </si>
+  <si>
     <t>Savant</t>
   </si>
   <si>
+    <t>02.07.2020 22:13:04</t>
+  </si>
+  <si>
+    <t>03:34</t>
+  </si>
+  <si>
+    <t>Desert Eagle</t>
+  </si>
+  <si>
     <t>Blind Guardian</t>
   </si>
   <si>
+    <t>20.07.2020 12:10:20</t>
+  </si>
+  <si>
+    <t>05:34</t>
+  </si>
+  <si>
+    <t>Nightfall</t>
+  </si>
+  <si>
+    <t>15.07.2020 22:13:04</t>
+  </si>
+  <si>
+    <t>07:12</t>
+  </si>
+  <si>
+    <t>Apocalypse</t>
+  </si>
+  <si>
+    <t>21.07.2020 04:40:40</t>
+  </si>
+  <si>
     <t>Infected Mushroom</t>
+  </si>
+  <si>
+    <t>XYZMusic</t>
+  </si>
+  <si>
+    <t>16.07.2020 01:13:15</t>
+  </si>
+  <si>
+    <t>06:06</t>
+  </si>
+  <si>
+    <t>Never Mind</t>
+  </si>
+  <si>
+    <t>15.07.2020 20:13:04</t>
+  </si>
+  <si>
+    <t>04:16</t>
+  </si>
+  <si>
+    <t>The Beginning Is Near</t>
+  </si>
+  <si>
+    <t>17.07.2020 02:13:15</t>
+  </si>
+  <si>
+    <t>15.07.2020 02:22:50</t>
+  </si>
+  <si>
+    <t>14.07.2020 02:21:15</t>
+  </si>
+  <si>
+    <t>01.07.2020 22:13:04</t>
+  </si>
+  <si>
+    <t>22.07.2020 12:12:12</t>
   </si>
 </sst>
 </file>
@@ -75,14 +162,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.86210060119629" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.826387405395508" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -90,6 +177,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="0" t="s">
         <v>1</v>
       </c>
     </row>
@@ -97,75 +196,255 @@
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="B4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>5</v>
+        <v>22</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>5</v>
+        <v>22</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="B12" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="B14" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create PieChart, BarChart class
</commit_message>
<xml_diff>
--- a/TrackAnalyser/TrackAnalyser/wwwroot/excel/Admin.xlsx
+++ b/TrackAnalyser/TrackAnalyser/wwwroot/excel/Admin.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Chars</t>
   </si>
@@ -20,10 +20,52 @@
     <t>Length</t>
   </si>
   <si>
+    <t>Iron Maiden</t>
+  </si>
+  <si>
+    <t>AntRadio</t>
+  </si>
+  <si>
+    <t>20.07.2020 02:10:30</t>
+  </si>
+  <si>
+    <t>04:32</t>
+  </si>
+  <si>
+    <t>Aces High</t>
+  </si>
+  <si>
+    <t>RadioS</t>
+  </si>
+  <si>
+    <t>19.07.2020 02:20:20</t>
+  </si>
+  <si>
+    <t>20.07.2020 02:12:30</t>
+  </si>
+  <si>
     <t>Savant</t>
   </si>
   <si>
-    <t>RadioS</t>
+    <t>02.07.2020 22:13:04</t>
+  </si>
+  <si>
+    <t>03:34</t>
+  </si>
+  <si>
+    <t>Desert Eagle</t>
+  </si>
+  <si>
+    <t>Blind Guardian</t>
+  </si>
+  <si>
+    <t>20.07.2020 12:10:20</t>
+  </si>
+  <si>
+    <t>05:34</t>
+  </si>
+  <si>
+    <t>Nightfall</t>
   </si>
   <si>
     <t>15.07.2020 22:13:04</t>
@@ -35,7 +77,46 @@
     <t>Apocalypse</t>
   </si>
   <si>
-    <t>AntRadio</t>
+    <t>21.07.2020 04:40:40</t>
+  </si>
+  <si>
+    <t>Infected Mushroom</t>
+  </si>
+  <si>
+    <t>XYZMusic</t>
+  </si>
+  <si>
+    <t>16.07.2020 01:13:15</t>
+  </si>
+  <si>
+    <t>06:06</t>
+  </si>
+  <si>
+    <t>Never Mind</t>
+  </si>
+  <si>
+    <t>15.07.2020 20:13:04</t>
+  </si>
+  <si>
+    <t>04:16</t>
+  </si>
+  <si>
+    <t>The Beginning Is Near</t>
+  </si>
+  <si>
+    <t>17.07.2020 02:13:15</t>
+  </si>
+  <si>
+    <t>15.07.2020 02:22:50</t>
+  </si>
+  <si>
+    <t>14.07.2020 02:21:15</t>
+  </si>
+  <si>
+    <t>01.07.2020 22:13:04</t>
+  </si>
+  <si>
+    <t>22.07.2020 12:12:12</t>
   </si>
 </sst>
 </file>
@@ -81,14 +162,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="9.489798545837402" customWidth="1"/>
+    <col min="1" max="1" width="18.86210060119629" customWidth="1"/>
+    <col min="2" max="2" width="9.826387405395508" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -136,13 +217,234 @@
         <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>